<commit_message>
Alvin updated some information.
</commit_message>
<xml_diff>
--- a/TestEnvironment.xlsx
+++ b/TestEnvironment.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="128">
   <si>
     <t>beta.esxi6.alv.pub</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +65,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>file.alv.pub</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>192.168.127.31</t>
   </si>
   <si>
@@ -103,13 +99,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rhel6.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.1.70</t>
-  </si>
-  <si>
     <t>alvin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,10 +168,6 @@
   </si>
   <si>
     <t>vcenter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nfs/samba</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1487,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1512,17 +1497,17 @@
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="8"/>
       <c r="B1" s="16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
       <c r="H1" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
@@ -1531,20 +1516,20 @@
     </row>
     <row r="2" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
@@ -1553,40 +1538,40 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1594,10 +1579,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="6">
         <v>8</v>
@@ -1606,7 +1591,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>1</v>
@@ -1621,21 +1606,21 @@
         <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6">
         <v>8</v>
@@ -1644,7 +1629,7 @@
         <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>1</v>
@@ -1659,10 +1644,10 @@
         <v>4</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1670,10 +1655,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6">
         <v>4</v>
@@ -1682,13 +1667,13 @@
         <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>7</v>
@@ -1697,10 +1682,10 @@
         <v>8</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1708,10 +1693,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -1720,19 +1705,19 @@
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="3"/>
@@ -1742,10 +1727,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -1754,19 +1739,19 @@
         <v>4</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="3"/>
@@ -1776,10 +1761,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3">
         <v>2</v>
@@ -1788,138 +1773,136 @@
         <v>4</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
       <c r="E11" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6">
         <v>2</v>
       </c>
-      <c r="E12" s="6">
-        <v>4</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="I12" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="D13" s="3">
         <v>4</v>
@@ -1928,32 +1911,32 @@
         <v>2</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3">
         <v>4</v>
@@ -1962,32 +1945,36 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D15" s="3">
         <v>4</v>
@@ -1996,152 +1983,150 @@
         <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="D16" s="3">
         <v>4</v>
       </c>
       <c r="E16" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="6">
+        <v>32</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="3">
-        <v>4</v>
-      </c>
-      <c r="E17" s="6">
-        <v>4</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="J17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="3">
+        <v>4</v>
+      </c>
+      <c r="E18" s="6">
+        <v>16</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
+      <c r="H18" s="6" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="3">
-        <v>8</v>
-      </c>
-      <c r="E18" s="6">
-        <v>32</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="D19" s="3">
         <v>4</v>
       </c>
       <c r="E19" s="6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>80</v>
@@ -2150,252 +2135,254 @@
         <v>3</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="K19" s="6"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D20" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E20" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>84</v>
+        <v>46</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D21" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E21" s="6">
-        <v>8</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>94</v>
+        <v>4</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="3">
-        <v>4</v>
-      </c>
-      <c r="E22" s="6">
-        <v>4</v>
-      </c>
-      <c r="F22" s="4" t="s">
+      <c r="D22" s="11">
+        <v>4</v>
+      </c>
+      <c r="E22" s="11">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="11">
+        <v>4</v>
+      </c>
+      <c r="E24" s="11">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="6">
+        <v>8</v>
+      </c>
+      <c r="E26" s="6">
+        <v>4</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="I26" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L22" s="6" t="s">
+      <c r="J26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B23" s="11" t="s">
+    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="11">
-        <v>4</v>
-      </c>
-      <c r="E23" s="11">
-        <v>1</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="11">
-        <v>4</v>
-      </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="D27" s="6">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E27" s="6">
         <v>4</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>119</v>
@@ -2404,13 +2391,13 @@
         <v>3</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -2418,11 +2405,11 @@
         <v>121</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>73</v>
-      </c>
       <c r="D28" s="6">
         <v>4</v>
       </c>
@@ -2430,200 +2417,162 @@
         <v>4</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L28" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="13">
+        <v>2</v>
+      </c>
+      <c r="E29" s="11">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="I29" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+    </row>
+    <row r="31" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="6">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6">
+        <v>4</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="6">
-        <v>4</v>
-      </c>
-      <c r="E29" s="6">
-        <v>4</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I29" s="6" t="s">
+      <c r="I31" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L29" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="13">
-        <v>2</v>
-      </c>
-      <c r="E30" s="11">
-        <v>1</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="J31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L31" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-    </row>
-    <row r="32" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="6">
-        <v>4</v>
-      </c>
-      <c r="E32" s="6">
-        <v>4</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L23" r:id="rId1"/>
+    <hyperlink ref="L22" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>